<commit_message>
Tweak to Excel format.
</commit_message>
<xml_diff>
--- a/tests/test1/output/main-recording.xlsx
+++ b/tests/test1/output/main-recording.xlsx
@@ -64,7 +64,7 @@
     <x:t>David</x:t>
   </x:si>
   <x:si>
-    <x:t>ViVI</x:t>
+    <x:t>mqrG</x:t>
   </x:si>
   <x:si>
     <x:t>Recorded</x:t>
@@ -85,7 +85,7 @@
     <x:t>quietly</x:t>
   </x:si>
   <x:si>
-    <x:t>b0aX</x:t>
+    <x:t>jnBw</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Part4_F0PF</x:t>
@@ -97,12 +97,11 @@
     <x:t>Go right!</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">There is a choice here.
-OPTION "Go right"
+    <x:t xml:space="preserve">OPTION "Go right"
 </x:t>
   </x:si>
   <x:si>
-    <x:t>hyEM</x:t>
+    <x:t>qidl</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Part4_DNII</x:t>
@@ -115,7 +114,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>YiSO</x:t>
+    <x:t>SUNv</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Part4_AJDP</x:t>
@@ -128,7 +127,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>Zy0S</x:t>
+    <x:t>D84D</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Part4_0YY1</x:t>
@@ -144,7 +143,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>tSLO</x:t>
+    <x:t>EoTA</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Right_WM69</x:t>
@@ -159,7 +158,7 @@
     <x:t>upset</x:t>
   </x:si>
   <x:si>
-    <x:t>Mvm7</x:t>
+    <x:t>Gcb0</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Left_MIM6</x:t>
@@ -171,7 +170,7 @@
     <x:t>You sure you want to go left?</x:t>
   </x:si>
   <x:si>
-    <x:t>mA8L</x:t>
+    <x:t>Zeqp</x:t>
   </x:si>
   <x:si>
     <x:t>main_TestScene_16U4</x:t>
@@ -186,13 +185,11 @@
     <x:t>This is a line I am saying.</x:t>
   </x:si>
   <x:si>
-    <x:t>This comment should apply to Test Scene.
-And so should this.
-Comment for a line.
+    <x:t>Comment for a line.
 Another comment for the same line.</x:t>
   </x:si>
   <x:si>
-    <x:t>SETw</x:t>
+    <x:t>aWNi</x:t>
   </x:si>
   <x:si>
     <x:t>Scratch</x:t>
@@ -237,11 +234,11 @@
     <x:t>Bark1</x:t>
   </x:si>
   <x:si>
-    <x:t>This is for all the barks.
-(1/7) This is for the one-legged version.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>8wYj</x:t>
+    <x:t xml:space="preserve">This is for all the barks.
+(1/7) </x:t>
+  </x:si>
+  <x:si>
+    <x:t>Ivci</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_UWZ2</x:t>
@@ -253,7 +250,7 @@
     <x:t xml:space="preserve">(2/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>iwh8</x:t>
+    <x:t>ZZCv</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_1ZG8</x:t>
@@ -262,10 +259,10 @@
     <x:t>Bark3</x:t>
   </x:si>
   <x:si>
-    <x:t>(3/7) How about this?</x:t>
-  </x:si>
-  <x:si>
-    <x:t>UvrK</x:t>
+    <x:t xml:space="preserve">(3/7) </x:t>
+  </x:si>
+  <x:si>
+    <x:t>gQ3M</x:t>
   </x:si>
   <x:si>
     <x:t>vo:soft, vo:radio</x:t>
@@ -280,7 +277,7 @@
     <x:t xml:space="preserve">(5/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>M3Ap</x:t>
+    <x:t>JpmJ</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_X291</x:t>
@@ -307,7 +304,7 @@
     <x:t xml:space="preserve">(6/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>Pk5H</x:t>
+    <x:t>Bun9</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_N07F</x:t>
@@ -319,7 +316,7 @@
     <x:t xml:space="preserve">(7/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>OZBd</x:t>
+    <x:t>Fken</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_7ZMT</x:t>
@@ -331,7 +328,7 @@
     <x:t>This is a recording line.</x:t>
   </x:si>
   <x:si>
-    <x:t>KjQI</x:t>
+    <x:t>QpWE</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartA_U9ZN</x:t>
@@ -343,7 +340,7 @@
     <x:t>This is a line hidden by a false clause.</x:t>
   </x:si>
   <x:si>
-    <x:t>wRQW</x:t>
+    <x:t>MQGj</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartB_VPX8</x:t>
@@ -358,7 +355,7 @@
     <x:t xml:space="preserve">(1/3) </x:t>
   </x:si>
   <x:si>
-    <x:t>7pM9</x:t>
+    <x:t>5hEN</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartB_FH4U</x:t>
@@ -367,7 +364,7 @@
     <x:t xml:space="preserve">(2/3) </x:t>
   </x:si>
   <x:si>
-    <x:t>6IVI</x:t>
+    <x:t>yV9X</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartB_1RQS</x:t>
@@ -379,7 +376,7 @@
     <x:t xml:space="preserve">(3/3) </x:t>
   </x:si>
   <x:si>
-    <x:t>k5XG</x:t>
+    <x:t>lfUb</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartC_JITN</x:t>
@@ -395,7 +392,7 @@
 (1/4) </x:t>
   </x:si>
   <x:si>
-    <x:t>V4Wh</x:t>
+    <x:t>pZwi</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartC_GUS9</x:t>
@@ -407,7 +404,7 @@
     <x:t xml:space="preserve">(2/4) </x:t>
   </x:si>
   <x:si>
-    <x:t>HZkD</x:t>
+    <x:t>qxob</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartC_3VZB</x:t>
@@ -419,7 +416,7 @@
     <x:t xml:space="preserve">(3/4) </x:t>
   </x:si>
   <x:si>
-    <x:t>OLBu</x:t>
+    <x:t>tc8C</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartC_A18G</x:t>
@@ -431,7 +428,7 @@
     <x:t xml:space="preserve">(4/4) </x:t>
   </x:si>
   <x:si>
-    <x:t>UX92</x:t>
+    <x:t>68Sc</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartD_UC9D</x:t>
@@ -440,13 +437,13 @@
     <x:t>Recording_PartD</x:t>
   </x:si>
   <x:si>
-    <x:t>al4B</x:t>
+    <x:t>E5ZZ</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartD_08WO</x:t>
   </x:si>
   <x:si>
-    <x:t>DXz9</x:t>
+    <x:t>anrS</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartE_81AO</x:t>
@@ -458,7 +455,7 @@
     <x:t>Goodbye!</x:t>
   </x:si>
   <x:si>
-    <x:t>lrJo</x:t>
+    <x:t>pIFe</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartE_JY1W</x:t>
@@ -467,7 +464,7 @@
     <x:t>Seeya!</x:t>
   </x:si>
   <x:si>
-    <x:t>86Hm</x:t>
+    <x:t>Vvby</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartE_QEM8</x:t>
@@ -476,7 +473,7 @@
     <x:t>Whoops!</x:t>
   </x:si>
   <x:si>
-    <x:t>vEFY</x:t>
+    <x:t>sQuy</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartE_KABN</x:t>
@@ -494,7 +491,7 @@
     <x:t>This is a conversation.</x:t>
   </x:si>
   <x:si>
-    <x:t>AajE</x:t>
+    <x:t>yZTD</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Branches_YTUY</x:t>
@@ -516,7 +513,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>8RXF</x:t>
+    <x:t>tQ7q</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Branches_PACN</x:t>
@@ -535,7 +532,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>Bi4R</x:t>
+    <x:t>Mtbr</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Branches_9ZRB</x:t>
@@ -550,7 +547,7 @@
     <x:t>Anyway, cold in here isn't it.</x:t>
   </x:si>
   <x:si>
-    <x:t>yyAI</x:t>
+    <x:t>lMbn</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Branches_6B6A</x:t>
@@ -568,7 +565,7 @@
     <x:t>I want to talk about the big room.</x:t>
   </x:si>
   <x:si>
-    <x:t>JrNK</x:t>
+    <x:t>wRVG</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Branches_BigRoom_GPMN</x:t>
@@ -586,7 +583,7 @@
     <x:t>I want to talk about the small room.</x:t>
   </x:si>
   <x:si>
-    <x:t>z87I</x:t>
+    <x:t>NVPq</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Branches_SmallRoom_413C</x:t>
@@ -607,7 +604,7 @@
     <x:t>Any more questions?</x:t>
   </x:si>
   <x:si>
-    <x:t>XDVJ</x:t>
+    <x:t>LUnl</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Branches_Hub_UYYD</x:t>
@@ -620,7 +617,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>7pR2</x:t>
+    <x:t>hiPf</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Branches_Hub_A048</x:t>
@@ -639,7 +636,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>RExl</x:t>
+    <x:t>ShN2</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Branches_Hub_Z1BD</x:t>
@@ -657,7 +654,7 @@
     <x:t>Is there something bigger?</x:t>
   </x:si>
   <x:si>
-    <x:t>X89o</x:t>
+    <x:t>6hRb</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Branches_Bigger_MFAH</x:t>
@@ -681,7 +678,7 @@
     <x:t>I am the colour of night.</x:t>
   </x:si>
   <x:si>
-    <x:t>6vTn</x:t>
+    <x:t>s5iM</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Flow_EPML</x:t>
@@ -696,7 +693,7 @@
     <x:t>Branch 1.</x:t>
   </x:si>
   <x:si>
-    <x:t>OQQQ</x:t>
+    <x:t>cpha</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Flow_IGPY</x:t>
@@ -705,7 +702,7 @@
     <x:t>Branch 2.</x:t>
   </x:si>
   <x:si>
-    <x:t>VXjF</x:t>
+    <x:t>qeo2</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Flow_QCX4</x:t>
@@ -714,7 +711,7 @@
     <x:t>Branch 3.</x:t>
   </x:si>
   <x:si>
-    <x:t>dh6W</x:t>
+    <x:t>G4JV</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Flow_EEQU</x:t>
@@ -723,7 +720,7 @@
     <x:t>And we're back.</x:t>
   </x:si>
   <x:si>
-    <x:t>r2CR</x:t>
+    <x:t>TFED</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -1163,7 +1160,7 @@
     <x:col min="3" max="3" width="11.210625" style="1" customWidth="1"/>
     <x:col min="4" max="4" width="35.710625" style="1" customWidth="1"/>
     <x:col min="5" max="5" width="10.335625" style="1" customWidth="1"/>
-    <x:col min="6" max="6" width="36.835625" style="1" customWidth="1"/>
+    <x:col min="6" max="6" width="32.960625" style="1" customWidth="1"/>
     <x:col min="7" max="7" width="7.460625" style="1" customWidth="1"/>
     <x:col min="8" max="8" width="11.210625" style="1" customWidth="1"/>
     <x:col min="9" max="9" width="14.335625" style="1" customWidth="1"/>
@@ -1266,7 +1263,7 @@
         <x:v>17</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:10" ht="27" customHeight="1" s="2" customFormat="1">
+    <x:row r="4" spans="1:10" ht="13.5" customHeight="1" s="2" customFormat="1">
       <x:c r="A4" s="2" t="s">
         <x:v>24</x:v>
       </x:c>
@@ -1458,7 +1455,7 @@
         <x:v>17</x:v>
       </x:c>
     </x:row>
-    <x:row r="10" spans="1:10" ht="54" customHeight="1" s="2" customFormat="1">
+    <x:row r="10" spans="1:10" ht="27" customHeight="1" s="2" customFormat="1">
       <x:c r="A10" s="2" t="s">
         <x:v>51</x:v>
       </x:c>

</xml_diff>

<commit_message>
Another fix to Excel format.
</commit_message>
<xml_diff>
--- a/tests/test1/output/main-recording.xlsx
+++ b/tests/test1/output/main-recording.xlsx
@@ -64,7 +64,7 @@
     <x:t>David</x:t>
   </x:si>
   <x:si>
-    <x:t>mqrG</x:t>
+    <x:t>C0we</x:t>
   </x:si>
   <x:si>
     <x:t>Recorded</x:t>
@@ -85,7 +85,7 @@
     <x:t>quietly</x:t>
   </x:si>
   <x:si>
-    <x:t>jnBw</x:t>
+    <x:t>XWzG</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Part4_F0PF</x:t>
@@ -101,7 +101,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>qidl</x:t>
+    <x:t>Ybb2</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Part4_DNII</x:t>
@@ -114,7 +114,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>SUNv</x:t>
+    <x:t>HKGk</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Part4_AJDP</x:t>
@@ -127,7 +127,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>D84D</x:t>
+    <x:t>Sh3Q</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Part4_0YY1</x:t>
@@ -143,7 +143,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>EoTA</x:t>
+    <x:t>pxHZ</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Right_WM69</x:t>
@@ -158,7 +158,7 @@
     <x:t>upset</x:t>
   </x:si>
   <x:si>
-    <x:t>Gcb0</x:t>
+    <x:t>AmGD</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Left_MIM6</x:t>
@@ -170,7 +170,7 @@
     <x:t>You sure you want to go left?</x:t>
   </x:si>
   <x:si>
-    <x:t>Zeqp</x:t>
+    <x:t>fvYr</x:t>
   </x:si>
   <x:si>
     <x:t>main_TestScene_16U4</x:t>
@@ -189,7 +189,7 @@
 Another comment for the same line.</x:t>
   </x:si>
   <x:si>
-    <x:t>aWNi</x:t>
+    <x:t>mt8K</x:t>
   </x:si>
   <x:si>
     <x:t>Scratch</x:t>
@@ -238,7 +238,7 @@
 (1/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>Ivci</x:t>
+    <x:t>OFVv</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_UWZ2</x:t>
@@ -250,7 +250,7 @@
     <x:t xml:space="preserve">(2/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>ZZCv</x:t>
+    <x:t>RueP</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_1ZG8</x:t>
@@ -262,7 +262,7 @@
     <x:t xml:space="preserve">(3/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>gQ3M</x:t>
+    <x:t>HXmO</x:t>
   </x:si>
   <x:si>
     <x:t>vo:soft, vo:radio</x:t>
@@ -277,7 +277,7 @@
     <x:t xml:space="preserve">(5/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>JpmJ</x:t>
+    <x:t>USeo</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_X291</x:t>
@@ -304,7 +304,7 @@
     <x:t xml:space="preserve">(6/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>Bun9</x:t>
+    <x:t>4kY0</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_N07F</x:t>
@@ -316,7 +316,7 @@
     <x:t xml:space="preserve">(7/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>Fken</x:t>
+    <x:t>P4EH</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_7ZMT</x:t>
@@ -328,7 +328,7 @@
     <x:t>This is a recording line.</x:t>
   </x:si>
   <x:si>
-    <x:t>QpWE</x:t>
+    <x:t>WLo1</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartA_U9ZN</x:t>
@@ -340,7 +340,7 @@
     <x:t>This is a line hidden by a false clause.</x:t>
   </x:si>
   <x:si>
-    <x:t>MQGj</x:t>
+    <x:t>8sXy</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartB_VPX8</x:t>
@@ -355,7 +355,7 @@
     <x:t xml:space="preserve">(1/3) </x:t>
   </x:si>
   <x:si>
-    <x:t>5hEN</x:t>
+    <x:t>tjx4</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartB_FH4U</x:t>
@@ -364,7 +364,7 @@
     <x:t xml:space="preserve">(2/3) </x:t>
   </x:si>
   <x:si>
-    <x:t>yV9X</x:t>
+    <x:t>160K</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartB_1RQS</x:t>
@@ -376,7 +376,7 @@
     <x:t xml:space="preserve">(3/3) </x:t>
   </x:si>
   <x:si>
-    <x:t>lfUb</x:t>
+    <x:t>fLoy</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartC_JITN</x:t>
@@ -392,7 +392,7 @@
 (1/4) </x:t>
   </x:si>
   <x:si>
-    <x:t>pZwi</x:t>
+    <x:t>5Whw</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartC_GUS9</x:t>
@@ -404,7 +404,7 @@
     <x:t xml:space="preserve">(2/4) </x:t>
   </x:si>
   <x:si>
-    <x:t>qxob</x:t>
+    <x:t>IZEZ</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartC_3VZB</x:t>
@@ -416,7 +416,7 @@
     <x:t xml:space="preserve">(3/4) </x:t>
   </x:si>
   <x:si>
-    <x:t>tc8C</x:t>
+    <x:t>u93M</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartC_A18G</x:t>
@@ -428,7 +428,7 @@
     <x:t xml:space="preserve">(4/4) </x:t>
   </x:si>
   <x:si>
-    <x:t>68Sc</x:t>
+    <x:t>Lod8</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartD_UC9D</x:t>
@@ -437,13 +437,13 @@
     <x:t>Recording_PartD</x:t>
   </x:si>
   <x:si>
-    <x:t>E5ZZ</x:t>
+    <x:t>JsZd</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartD_08WO</x:t>
   </x:si>
   <x:si>
-    <x:t>anrS</x:t>
+    <x:t>QAMU</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartE_81AO</x:t>
@@ -455,7 +455,7 @@
     <x:t>Goodbye!</x:t>
   </x:si>
   <x:si>
-    <x:t>pIFe</x:t>
+    <x:t>zce2</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartE_JY1W</x:t>
@@ -464,7 +464,7 @@
     <x:t>Seeya!</x:t>
   </x:si>
   <x:si>
-    <x:t>Vvby</x:t>
+    <x:t>1SpY</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartE_QEM8</x:t>
@@ -473,7 +473,7 @@
     <x:t>Whoops!</x:t>
   </x:si>
   <x:si>
-    <x:t>sQuy</x:t>
+    <x:t>jZbE</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartE_KABN</x:t>
@@ -491,7 +491,7 @@
     <x:t>This is a conversation.</x:t>
   </x:si>
   <x:si>
-    <x:t>yZTD</x:t>
+    <x:t>JYwS</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Branches_YTUY</x:t>
@@ -513,7 +513,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>tQ7q</x:t>
+    <x:t>ADPB</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Branches_PACN</x:t>
@@ -532,7 +532,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>Mtbr</x:t>
+    <x:t>qO8z</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Branches_9ZRB</x:t>
@@ -547,7 +547,7 @@
     <x:t>Anyway, cold in here isn't it.</x:t>
   </x:si>
   <x:si>
-    <x:t>lMbn</x:t>
+    <x:t>DIaz</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Branches_6B6A</x:t>
@@ -565,7 +565,7 @@
     <x:t>I want to talk about the big room.</x:t>
   </x:si>
   <x:si>
-    <x:t>wRVG</x:t>
+    <x:t>jVVR</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Branches_BigRoom_GPMN</x:t>
@@ -583,7 +583,7 @@
     <x:t>I want to talk about the small room.</x:t>
   </x:si>
   <x:si>
-    <x:t>NVPq</x:t>
+    <x:t>Vv8j</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Branches_SmallRoom_413C</x:t>
@@ -604,7 +604,7 @@
     <x:t>Any more questions?</x:t>
   </x:si>
   <x:si>
-    <x:t>LUnl</x:t>
+    <x:t>C2nI</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Branches_Hub_UYYD</x:t>
@@ -617,7 +617,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>hiPf</x:t>
+    <x:t>CROF</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Branches_Hub_A048</x:t>
@@ -636,7 +636,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>ShN2</x:t>
+    <x:t>2Qsx</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Branches_Hub_Z1BD</x:t>
@@ -654,7 +654,7 @@
     <x:t>Is there something bigger?</x:t>
   </x:si>
   <x:si>
-    <x:t>6hRb</x:t>
+    <x:t>SJs5</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Branches_Bigger_MFAH</x:t>
@@ -678,7 +678,7 @@
     <x:t>I am the colour of night.</x:t>
   </x:si>
   <x:si>
-    <x:t>s5iM</x:t>
+    <x:t>fJMF</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Flow_EPML</x:t>
@@ -693,7 +693,7 @@
     <x:t>Branch 1.</x:t>
   </x:si>
   <x:si>
-    <x:t>cpha</x:t>
+    <x:t>lJ7z</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Flow_IGPY</x:t>
@@ -702,7 +702,7 @@
     <x:t>Branch 2.</x:t>
   </x:si>
   <x:si>
-    <x:t>qeo2</x:t>
+    <x:t>6fvy</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Flow_QCX4</x:t>
@@ -711,7 +711,7 @@
     <x:t>Branch 3.</x:t>
   </x:si>
   <x:si>
-    <x:t>G4JV</x:t>
+    <x:t>Bmd5</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Flow_EEQU</x:t>
@@ -720,7 +720,7 @@
     <x:t>And we're back.</x:t>
   </x:si>
   <x:si>
-    <x:t>TFED</x:t>
+    <x:t>E3wK</x:t>
   </x:si>
 </x:sst>
 </file>

</xml_diff>

<commit_message>
Added ignore error types to Excel writing.
</commit_message>
<xml_diff>
--- a/tests/test1/output/main-recording.xlsx
+++ b/tests/test1/output/main-recording.xlsx
@@ -64,7 +64,7 @@
     <x:t>David</x:t>
   </x:si>
   <x:si>
-    <x:t>C0we</x:t>
+    <x:t>OhHQ</x:t>
   </x:si>
   <x:si>
     <x:t>Recorded</x:t>
@@ -85,7 +85,7 @@
     <x:t>quietly</x:t>
   </x:si>
   <x:si>
-    <x:t>XWzG</x:t>
+    <x:t>nclm</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Part4_F0PF</x:t>
@@ -101,7 +101,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>Ybb2</x:t>
+    <x:t>D2th</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Part4_DNII</x:t>
@@ -114,7 +114,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>HKGk</x:t>
+    <x:t>JFUC</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Part4_AJDP</x:t>
@@ -127,7 +127,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>Sh3Q</x:t>
+    <x:t>QNYz</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Part4_0YY1</x:t>
@@ -143,7 +143,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>pxHZ</x:t>
+    <x:t>0k3Z</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Right_WM69</x:t>
@@ -158,7 +158,7 @@
     <x:t>upset</x:t>
   </x:si>
   <x:si>
-    <x:t>AmGD</x:t>
+    <x:t>PWyz</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Left_MIM6</x:t>
@@ -170,7 +170,7 @@
     <x:t>You sure you want to go left?</x:t>
   </x:si>
   <x:si>
-    <x:t>fvYr</x:t>
+    <x:t>nitE</x:t>
   </x:si>
   <x:si>
     <x:t>main_TestScene_16U4</x:t>
@@ -189,7 +189,7 @@
 Another comment for the same line.</x:t>
   </x:si>
   <x:si>
-    <x:t>mt8K</x:t>
+    <x:t>kMK7</x:t>
   </x:si>
   <x:si>
     <x:t>Scratch</x:t>
@@ -238,7 +238,7 @@
 (1/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>OFVv</x:t>
+    <x:t>ecfI</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_UWZ2</x:t>
@@ -250,7 +250,7 @@
     <x:t xml:space="preserve">(2/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>RueP</x:t>
+    <x:t>JmRQ</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_1ZG8</x:t>
@@ -262,7 +262,7 @@
     <x:t xml:space="preserve">(3/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>HXmO</x:t>
+    <x:t>4w0N</x:t>
   </x:si>
   <x:si>
     <x:t>vo:soft, vo:radio</x:t>
@@ -277,7 +277,7 @@
     <x:t xml:space="preserve">(5/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>USeo</x:t>
+    <x:t>9GKb</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_X291</x:t>
@@ -304,7 +304,7 @@
     <x:t xml:space="preserve">(6/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>4kY0</x:t>
+    <x:t>10zC</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_N07F</x:t>
@@ -316,7 +316,7 @@
     <x:t xml:space="preserve">(7/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>P4EH</x:t>
+    <x:t>vdQu</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_7ZMT</x:t>
@@ -328,7 +328,7 @@
     <x:t>This is a recording line.</x:t>
   </x:si>
   <x:si>
-    <x:t>WLo1</x:t>
+    <x:t>44tN</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartA_U9ZN</x:t>
@@ -340,7 +340,7 @@
     <x:t>This is a line hidden by a false clause.</x:t>
   </x:si>
   <x:si>
-    <x:t>8sXy</x:t>
+    <x:t>vbL0</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartB_VPX8</x:t>
@@ -355,7 +355,7 @@
     <x:t xml:space="preserve">(1/3) </x:t>
   </x:si>
   <x:si>
-    <x:t>tjx4</x:t>
+    <x:t>rclH</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartB_FH4U</x:t>
@@ -364,7 +364,7 @@
     <x:t xml:space="preserve">(2/3) </x:t>
   </x:si>
   <x:si>
-    <x:t>160K</x:t>
+    <x:t>3avX</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartB_1RQS</x:t>
@@ -376,7 +376,7 @@
     <x:t xml:space="preserve">(3/3) </x:t>
   </x:si>
   <x:si>
-    <x:t>fLoy</x:t>
+    <x:t>ak9g</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartC_JITN</x:t>
@@ -392,7 +392,7 @@
 (1/4) </x:t>
   </x:si>
   <x:si>
-    <x:t>5Whw</x:t>
+    <x:t>dWrP</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartC_GUS9</x:t>
@@ -404,7 +404,7 @@
     <x:t xml:space="preserve">(2/4) </x:t>
   </x:si>
   <x:si>
-    <x:t>IZEZ</x:t>
+    <x:t>oKQv</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartC_3VZB</x:t>
@@ -416,7 +416,7 @@
     <x:t xml:space="preserve">(3/4) </x:t>
   </x:si>
   <x:si>
-    <x:t>u93M</x:t>
+    <x:t>K3dT</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartC_A18G</x:t>
@@ -428,7 +428,7 @@
     <x:t xml:space="preserve">(4/4) </x:t>
   </x:si>
   <x:si>
-    <x:t>Lod8</x:t>
+    <x:t>86MY</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartD_UC9D</x:t>
@@ -437,13 +437,13 @@
     <x:t>Recording_PartD</x:t>
   </x:si>
   <x:si>
-    <x:t>JsZd</x:t>
+    <x:t>B8Oc</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartD_08WO</x:t>
   </x:si>
   <x:si>
-    <x:t>QAMU</x:t>
+    <x:t>RBTG</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartE_81AO</x:t>
@@ -455,7 +455,7 @@
     <x:t>Goodbye!</x:t>
   </x:si>
   <x:si>
-    <x:t>zce2</x:t>
+    <x:t>a7Xy</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartE_JY1W</x:t>
@@ -464,7 +464,7 @@
     <x:t>Seeya!</x:t>
   </x:si>
   <x:si>
-    <x:t>1SpY</x:t>
+    <x:t>zzHC</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartE_QEM8</x:t>
@@ -473,7 +473,7 @@
     <x:t>Whoops!</x:t>
   </x:si>
   <x:si>
-    <x:t>jZbE</x:t>
+    <x:t>mKpa</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartE_KABN</x:t>
@@ -491,7 +491,7 @@
     <x:t>This is a conversation.</x:t>
   </x:si>
   <x:si>
-    <x:t>JYwS</x:t>
+    <x:t>mxtg</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Branches_YTUY</x:t>
@@ -513,7 +513,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>ADPB</x:t>
+    <x:t>tBXh</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Branches_PACN</x:t>
@@ -532,7 +532,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>qO8z</x:t>
+    <x:t>D0vq</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Branches_9ZRB</x:t>
@@ -547,7 +547,7 @@
     <x:t>Anyway, cold in here isn't it.</x:t>
   </x:si>
   <x:si>
-    <x:t>DIaz</x:t>
+    <x:t>EwkS</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Branches_6B6A</x:t>
@@ -565,7 +565,7 @@
     <x:t>I want to talk about the big room.</x:t>
   </x:si>
   <x:si>
-    <x:t>jVVR</x:t>
+    <x:t>0OHN</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Branches_BigRoom_GPMN</x:t>
@@ -583,7 +583,7 @@
     <x:t>I want to talk about the small room.</x:t>
   </x:si>
   <x:si>
-    <x:t>Vv8j</x:t>
+    <x:t>lrKl</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Branches_SmallRoom_413C</x:t>
@@ -604,7 +604,7 @@
     <x:t>Any more questions?</x:t>
   </x:si>
   <x:si>
-    <x:t>C2nI</x:t>
+    <x:t>vu9c</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Branches_Hub_UYYD</x:t>
@@ -617,7 +617,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>CROF</x:t>
+    <x:t>CmDv</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Branches_Hub_A048</x:t>
@@ -636,7 +636,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>2Qsx</x:t>
+    <x:t>p85p</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Branches_Hub_Z1BD</x:t>
@@ -654,7 +654,7 @@
     <x:t>Is there something bigger?</x:t>
   </x:si>
   <x:si>
-    <x:t>SJs5</x:t>
+    <x:t>RwXH</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Branches_Bigger_MFAH</x:t>
@@ -678,7 +678,7 @@
     <x:t>I am the colour of night.</x:t>
   </x:si>
   <x:si>
-    <x:t>fJMF</x:t>
+    <x:t>bSwY</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Flow_EPML</x:t>
@@ -693,7 +693,7 @@
     <x:t>Branch 1.</x:t>
   </x:si>
   <x:si>
-    <x:t>lJ7z</x:t>
+    <x:t>0g6w</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Flow_IGPY</x:t>
@@ -702,7 +702,7 @@
     <x:t>Branch 2.</x:t>
   </x:si>
   <x:si>
-    <x:t>6fvy</x:t>
+    <x:t>X3jJ</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Flow_QCX4</x:t>
@@ -711,7 +711,7 @@
     <x:t>Branch 3.</x:t>
   </x:si>
   <x:si>
-    <x:t>Bmd5</x:t>
+    <x:t>D6Bb</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Flow_EEQU</x:t>
@@ -720,7 +720,7 @@
     <x:t>And we're back.</x:t>
   </x:si>
   <x:si>
-    <x:t>E3wK</x:t>
+    <x:t>Ed2a</x:t>
   </x:si>
 </x:sst>
 </file>

</xml_diff>

<commit_message>
Try a new strategy for the Excel format issue.
</commit_message>
<xml_diff>
--- a/tests/test1/output/main-recording.xlsx
+++ b/tests/test1/output/main-recording.xlsx
@@ -64,7 +64,7 @@
     <x:t>David</x:t>
   </x:si>
   <x:si>
-    <x:t>OhHQ</x:t>
+    <x:t>Uboh</x:t>
   </x:si>
   <x:si>
     <x:t>Recorded</x:t>
@@ -85,7 +85,7 @@
     <x:t>quietly</x:t>
   </x:si>
   <x:si>
-    <x:t>nclm</x:t>
+    <x:t>h2eg</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Part4_F0PF</x:t>
@@ -101,7 +101,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>D2th</x:t>
+    <x:t>HLVR</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Part4_DNII</x:t>
@@ -114,7 +114,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>JFUC</x:t>
+    <x:t>qCE6</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Part4_AJDP</x:t>
@@ -127,7 +127,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>QNYz</x:t>
+    <x:t>1Y8A</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Part4_0YY1</x:t>
@@ -143,7 +143,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>0k3Z</x:t>
+    <x:t>Ry2W</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Right_WM69</x:t>
@@ -158,7 +158,7 @@
     <x:t>upset</x:t>
   </x:si>
   <x:si>
-    <x:t>PWyz</x:t>
+    <x:t>Swb0</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Left_MIM6</x:t>
@@ -170,7 +170,7 @@
     <x:t>You sure you want to go left?</x:t>
   </x:si>
   <x:si>
-    <x:t>nitE</x:t>
+    <x:t>GjFV</x:t>
   </x:si>
   <x:si>
     <x:t>main_TestScene_16U4</x:t>
@@ -189,7 +189,7 @@
 Another comment for the same line.</x:t>
   </x:si>
   <x:si>
-    <x:t>kMK7</x:t>
+    <x:t>Ibtw</x:t>
   </x:si>
   <x:si>
     <x:t>Scratch</x:t>
@@ -238,7 +238,7 @@
 (1/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>ecfI</x:t>
+    <x:t>w0Sk</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_UWZ2</x:t>
@@ -250,7 +250,7 @@
     <x:t xml:space="preserve">(2/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>JmRQ</x:t>
+    <x:t>5Cz6</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_1ZG8</x:t>
@@ -262,7 +262,7 @@
     <x:t xml:space="preserve">(3/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>4w0N</x:t>
+    <x:t>YnCs</x:t>
   </x:si>
   <x:si>
     <x:t>vo:soft, vo:radio</x:t>
@@ -277,7 +277,7 @@
     <x:t xml:space="preserve">(5/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>9GKb</x:t>
+    <x:t>7ASK</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_X291</x:t>
@@ -304,7 +304,7 @@
     <x:t xml:space="preserve">(6/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>10zC</x:t>
+    <x:t>zuUX</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_N07F</x:t>
@@ -316,7 +316,7 @@
     <x:t xml:space="preserve">(7/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>vdQu</x:t>
+    <x:t>MK6X</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_7ZMT</x:t>
@@ -328,7 +328,7 @@
     <x:t>This is a recording line.</x:t>
   </x:si>
   <x:si>
-    <x:t>44tN</x:t>
+    <x:t>i0Kg</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartA_U9ZN</x:t>
@@ -340,7 +340,7 @@
     <x:t>This is a line hidden by a false clause.</x:t>
   </x:si>
   <x:si>
-    <x:t>vbL0</x:t>
+    <x:t>FaBu</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartB_VPX8</x:t>
@@ -355,7 +355,7 @@
     <x:t xml:space="preserve">(1/3) </x:t>
   </x:si>
   <x:si>
-    <x:t>rclH</x:t>
+    <x:t>6ypN</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartB_FH4U</x:t>
@@ -364,7 +364,7 @@
     <x:t xml:space="preserve">(2/3) </x:t>
   </x:si>
   <x:si>
-    <x:t>3avX</x:t>
+    <x:t>qtLT</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartB_1RQS</x:t>
@@ -376,7 +376,7 @@
     <x:t xml:space="preserve">(3/3) </x:t>
   </x:si>
   <x:si>
-    <x:t>ak9g</x:t>
+    <x:t>sYCw</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartC_JITN</x:t>
@@ -392,7 +392,7 @@
 (1/4) </x:t>
   </x:si>
   <x:si>
-    <x:t>dWrP</x:t>
+    <x:t>M4ZR</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartC_GUS9</x:t>
@@ -404,7 +404,7 @@
     <x:t xml:space="preserve">(2/4) </x:t>
   </x:si>
   <x:si>
-    <x:t>oKQv</x:t>
+    <x:t>33ji</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartC_3VZB</x:t>
@@ -416,7 +416,7 @@
     <x:t xml:space="preserve">(3/4) </x:t>
   </x:si>
   <x:si>
-    <x:t>K3dT</x:t>
+    <x:t>W7YK</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartC_A18G</x:t>
@@ -428,7 +428,7 @@
     <x:t xml:space="preserve">(4/4) </x:t>
   </x:si>
   <x:si>
-    <x:t>86MY</x:t>
+    <x:t>sn1B</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartD_UC9D</x:t>
@@ -437,13 +437,13 @@
     <x:t>Recording_PartD</x:t>
   </x:si>
   <x:si>
-    <x:t>B8Oc</x:t>
+    <x:t>zPtx</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartD_08WO</x:t>
   </x:si>
   <x:si>
-    <x:t>RBTG</x:t>
+    <x:t>f8LK</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartE_81AO</x:t>
@@ -455,7 +455,7 @@
     <x:t>Goodbye!</x:t>
   </x:si>
   <x:si>
-    <x:t>a7Xy</x:t>
+    <x:t>pINk</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartE_JY1W</x:t>
@@ -464,7 +464,7 @@
     <x:t>Seeya!</x:t>
   </x:si>
   <x:si>
-    <x:t>zzHC</x:t>
+    <x:t>ONfP</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartE_QEM8</x:t>
@@ -473,7 +473,7 @@
     <x:t>Whoops!</x:t>
   </x:si>
   <x:si>
-    <x:t>mKpa</x:t>
+    <x:t>9Y1E</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartE_KABN</x:t>
@@ -491,7 +491,7 @@
     <x:t>This is a conversation.</x:t>
   </x:si>
   <x:si>
-    <x:t>mxtg</x:t>
+    <x:t>C2h0</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Branches_YTUY</x:t>
@@ -513,7 +513,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>tBXh</x:t>
+    <x:t>6E7M</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Branches_PACN</x:t>
@@ -532,7 +532,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>D0vq</x:t>
+    <x:t>2HPo</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Branches_9ZRB</x:t>
@@ -547,7 +547,7 @@
     <x:t>Anyway, cold in here isn't it.</x:t>
   </x:si>
   <x:si>
-    <x:t>EwkS</x:t>
+    <x:t>bhDy</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Branches_6B6A</x:t>
@@ -565,7 +565,7 @@
     <x:t>I want to talk about the big room.</x:t>
   </x:si>
   <x:si>
-    <x:t>0OHN</x:t>
+    <x:t>ORi7</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Branches_BigRoom_GPMN</x:t>
@@ -583,7 +583,7 @@
     <x:t>I want to talk about the small room.</x:t>
   </x:si>
   <x:si>
-    <x:t>lrKl</x:t>
+    <x:t>0rPJ</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Branches_SmallRoom_413C</x:t>
@@ -604,7 +604,7 @@
     <x:t>Any more questions?</x:t>
   </x:si>
   <x:si>
-    <x:t>vu9c</x:t>
+    <x:t>1Ysb</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Branches_Hub_UYYD</x:t>
@@ -617,7 +617,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>CmDv</x:t>
+    <x:t>uRBE</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Branches_Hub_A048</x:t>
@@ -636,7 +636,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>p85p</x:t>
+    <x:t>xoT7</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Branches_Hub_Z1BD</x:t>
@@ -654,7 +654,7 @@
     <x:t>Is there something bigger?</x:t>
   </x:si>
   <x:si>
-    <x:t>RwXH</x:t>
+    <x:t>HgC0</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Branches_Bigger_MFAH</x:t>
@@ -678,7 +678,7 @@
     <x:t>I am the colour of night.</x:t>
   </x:si>
   <x:si>
-    <x:t>bSwY</x:t>
+    <x:t>w4KQ</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Flow_EPML</x:t>
@@ -693,7 +693,7 @@
     <x:t>Branch 1.</x:t>
   </x:si>
   <x:si>
-    <x:t>0g6w</x:t>
+    <x:t>qdWm</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Flow_IGPY</x:t>
@@ -702,7 +702,7 @@
     <x:t>Branch 2.</x:t>
   </x:si>
   <x:si>
-    <x:t>X3jJ</x:t>
+    <x:t>p7nG</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Flow_QCX4</x:t>
@@ -711,7 +711,7 @@
     <x:t>Branch 3.</x:t>
   </x:si>
   <x:si>
-    <x:t>D6Bb</x:t>
+    <x:t>73iL</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Flow_EEQU</x:t>
@@ -720,7 +720,7 @@
     <x:t>And we're back.</x:t>
   </x:si>
   <x:si>
-    <x:t>Ed2a</x:t>
+    <x:t>7nV5</x:t>
   </x:si>
 </x:sst>
 </file>

</xml_diff>

<commit_message>
Remove requirement for square brackets.
</commit_message>
<xml_diff>
--- a/tests/test1/output/main-recording.xlsx
+++ b/tests/test1/output/main-recording.xlsx
@@ -65,7 +65,7 @@
 Another comment for the same line.</x:t>
   </x:si>
   <x:si>
-    <x:t>3zjn</x:t>
+    <x:t>oKmf</x:t>
   </x:si>
   <x:si>
     <x:t>Scratch</x:t>
@@ -120,7 +120,7 @@
 (1/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>9zI8</x:t>
+    <x:t>EWWw</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_UWZ2</x:t>
@@ -132,7 +132,7 @@
     <x:t xml:space="preserve">(2/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>3N9u</x:t>
+    <x:t>fkRB</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_1ZG8</x:t>
@@ -144,7 +144,7 @@
     <x:t xml:space="preserve">(3/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>IsM1</x:t>
+    <x:t>jw60</x:t>
   </x:si>
   <x:si>
     <x:t>vo:soft, vo:radio</x:t>
@@ -159,7 +159,7 @@
     <x:t xml:space="preserve">(5/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>kfUZ</x:t>
+    <x:t>n0GD</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_X291</x:t>
@@ -186,7 +186,7 @@
     <x:t xml:space="preserve">(6/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>KZ97</x:t>
+    <x:t>ScZx</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_N07F</x:t>
@@ -198,7 +198,7 @@
     <x:t xml:space="preserve">(7/7) </x:t>
   </x:si>
   <x:si>
-    <x:t>muSm</x:t>
+    <x:t>0HuQ</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_7ZMT</x:t>
@@ -210,7 +210,7 @@
     <x:t>This is a recording line.</x:t>
   </x:si>
   <x:si>
-    <x:t>hVmO</x:t>
+    <x:t>Fph3</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartA_U9ZN</x:t>
@@ -222,7 +222,7 @@
     <x:t>This is a line hidden by a false clause.</x:t>
   </x:si>
   <x:si>
-    <x:t>vTZz</x:t>
+    <x:t>5hE2</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartB_VPX8</x:t>
@@ -237,7 +237,7 @@
     <x:t xml:space="preserve">(1/3) </x:t>
   </x:si>
   <x:si>
-    <x:t>OWMg</x:t>
+    <x:t>5PeT</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartB_FH4U</x:t>
@@ -246,7 +246,7 @@
     <x:t xml:space="preserve">(2/3) </x:t>
   </x:si>
   <x:si>
-    <x:t>9n8S</x:t>
+    <x:t>9a3L</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartB_1RQS</x:t>
@@ -258,7 +258,7 @@
     <x:t xml:space="preserve">(3/3) </x:t>
   </x:si>
   <x:si>
-    <x:t>XQLH</x:t>
+    <x:t>wPIk</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartC_JITN</x:t>
@@ -274,7 +274,7 @@
 (1/4) </x:t>
   </x:si>
   <x:si>
-    <x:t>we9i</x:t>
+    <x:t>N2nj</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartC_GUS9</x:t>
@@ -286,7 +286,7 @@
     <x:t xml:space="preserve">(2/4) </x:t>
   </x:si>
   <x:si>
-    <x:t>TSPT</x:t>
+    <x:t>OYCT</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartC_3VZB</x:t>
@@ -298,7 +298,7 @@
     <x:t xml:space="preserve">(3/4) </x:t>
   </x:si>
   <x:si>
-    <x:t>RMKS</x:t>
+    <x:t>Rqfr</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartC_A18G</x:t>
@@ -310,7 +310,7 @@
     <x:t xml:space="preserve">(4/4) </x:t>
   </x:si>
   <x:si>
-    <x:t>8bAi</x:t>
+    <x:t>j2Eo</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartD_UC9D</x:t>
@@ -319,13 +319,13 @@
     <x:t>Recording_PartD</x:t>
   </x:si>
   <x:si>
-    <x:t>qANb</x:t>
+    <x:t>Vv9k</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartD_08WO</x:t>
   </x:si>
   <x:si>
-    <x:t>Hxzf</x:t>
+    <x:t>EDuz</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartE_81AO</x:t>
@@ -337,7 +337,7 @@
     <x:t>Goodbye!</x:t>
   </x:si>
   <x:si>
-    <x:t>OWWV</x:t>
+    <x:t>17Dg</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartE_JY1W</x:t>
@@ -346,7 +346,7 @@
     <x:t>Seeya!</x:t>
   </x:si>
   <x:si>
-    <x:t>dIsI</x:t>
+    <x:t>1xIF</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartE_QEM8</x:t>
@@ -355,7 +355,7 @@
     <x:t>Whoops!</x:t>
   </x:si>
   <x:si>
-    <x:t>c2w8</x:t>
+    <x:t>bGx0</x:t>
   </x:si>
   <x:si>
     <x:t>main_Recording_PartE_KABN</x:t>
@@ -373,7 +373,7 @@
     <x:t>This is a scene.</x:t>
   </x:si>
   <x:si>
-    <x:t>ub09</x:t>
+    <x:t>ugeS</x:t>
   </x:si>
   <x:si>
     <x:t>Recorded</x:t>
@@ -394,7 +394,7 @@
     <x:t>quietly</x:t>
   </x:si>
   <x:si>
-    <x:t>ILBj</x:t>
+    <x:t>rMi4</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Part4_F0PF</x:t>
@@ -410,7 +410,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>bBEF</x:t>
+    <x:t>Iu8v</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Part4_DNII</x:t>
@@ -423,7 +423,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>xVw4</x:t>
+    <x:t>N5Ua</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Part4_AJDP</x:t>
@@ -436,7 +436,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>WjKc</x:t>
+    <x:t>GvGO</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Part4_P46B</x:t>
@@ -448,7 +448,7 @@
     <x:t>OPTION "Trying dialogue here."</x:t>
   </x:si>
   <x:si>
-    <x:t>2S43</x:t>
+    <x:t>90Aj</x:t>
   </x:si>
   <x:si>
     <x:t>TTS</x:t>
@@ -472,7 +472,7 @@
     <x:t>OPTION "Trying dialogue with no line underneath."</x:t>
   </x:si>
   <x:si>
-    <x:t>FIr3</x:t>
+    <x:t>BLqx</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Part4_0YY1</x:t>
@@ -485,7 +485,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>6LB7</x:t>
+    <x:t>Zyoh</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Right_WM69</x:t>
@@ -500,7 +500,7 @@
     <x:t>upset</x:t>
   </x:si>
   <x:si>
-    <x:t>nWeU</x:t>
+    <x:t>mwR8</x:t>
   </x:si>
   <x:si>
     <x:t>scene1_Scene1_Left_MIM6</x:t>
@@ -512,7 +512,7 @@
     <x:t>You sure you want to go left?</x:t>
   </x:si>
   <x:si>
-    <x:t>QbbF</x:t>
+    <x:t>DiZp</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Branches_41YM</x:t>
@@ -524,7 +524,7 @@
     <x:t>This is a conversation.</x:t>
   </x:si>
   <x:si>
-    <x:t>gIuP</x:t>
+    <x:t>tWdz</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Branches_YTUY</x:t>
@@ -543,7 +543,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>G4Y4</x:t>
+    <x:t>vlAh</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Branches_PACN</x:t>
@@ -562,7 +562,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>pIIa</x:t>
+    <x:t>O2sZ</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Branches_9ZRB</x:t>
@@ -577,7 +577,7 @@
     <x:t>Anyway, cold in here isn't it.</x:t>
   </x:si>
   <x:si>
-    <x:t>lMC7</x:t>
+    <x:t>Klxp</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Branches_6B6A</x:t>
@@ -595,7 +595,7 @@
     <x:t>I want to talk about the big room.</x:t>
   </x:si>
   <x:si>
-    <x:t>mmW9</x:t>
+    <x:t>JLYX</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Branches_BigRoom_GPMN</x:t>
@@ -613,7 +613,7 @@
     <x:t>I want to talk about the small room.</x:t>
   </x:si>
   <x:si>
-    <x:t>29j9</x:t>
+    <x:t>43cO</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Branches_SmallRoom_413C</x:t>
@@ -634,7 +634,7 @@
     <x:t>Any more questions?</x:t>
   </x:si>
   <x:si>
-    <x:t>ZFOg</x:t>
+    <x:t>ZNMU</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Branches_Hub_UYYD</x:t>
@@ -647,7 +647,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>wRzh</x:t>
+    <x:t>tclJ</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Branches_Hub_A048</x:t>
@@ -666,7 +666,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>ONsL</x:t>
+    <x:t>DWQB</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Branches_Hub_Z1BD</x:t>
@@ -684,7 +684,7 @@
     <x:t>Is there something bigger?</x:t>
   </x:si>
   <x:si>
-    <x:t>w7KZ</x:t>
+    <x:t>DPh5</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Branches_Bigger_MFAH</x:t>
@@ -708,7 +708,7 @@
     <x:t>I am the colour of night.</x:t>
   </x:si>
   <x:si>
-    <x:t>LG5w</x:t>
+    <x:t>kukZ</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Flow_EPML</x:t>
@@ -723,7 +723,7 @@
     <x:t>Branch 1.</x:t>
   </x:si>
   <x:si>
-    <x:t>Ng2P</x:t>
+    <x:t>EDLn</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Flow_IGPY</x:t>
@@ -732,7 +732,7 @@
     <x:t>Branch 2.</x:t>
   </x:si>
   <x:si>
-    <x:t>0ezk</x:t>
+    <x:t>VVAn</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Flow_QCX4</x:t>
@@ -741,7 +741,7 @@
     <x:t>Branch 3.</x:t>
   </x:si>
   <x:si>
-    <x:t>NBfq</x:t>
+    <x:t>4xa0</x:t>
   </x:si>
   <x:si>
     <x:t>branches_Flow_EEQU</x:t>
@@ -750,7 +750,7 @@
     <x:t>And we're back.</x:t>
   </x:si>
   <x:si>
-    <x:t>BTMW</x:t>
+    <x:t>wVpR</x:t>
   </x:si>
 </x:sst>
 </file>

</xml_diff>